<commit_message>
Added first results to readme.
</commit_message>
<xml_diff>
--- a/Speed_second_run.xlsx
+++ b/Speed_second_run.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BE0574-9F82-410D-93B5-AD2EB4B85C38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531FA785-3F9E-42E9-BBF3-37529A43D8D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="7470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Changed Plain to Pure.
</commit_message>
<xml_diff>
--- a/Speed_second_run.xlsx
+++ b/Speed_second_run.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531FA785-3F9E-42E9-BBF3-37529A43D8D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFB1AC8-8BCB-4C06-8B40-FD325B003C9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="7470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,25 +28,16 @@
     <t>adopt-imaging-single</t>
   </si>
   <si>
-    <t>adopt-plain</t>
-  </si>
-  <si>
     <t>amazoncorretto-imaging-parallel</t>
   </si>
   <si>
     <t>amazoncorretto-imaging-single</t>
   </si>
   <si>
-    <t>amazoncorretto-plain</t>
-  </si>
-  <si>
     <t>graaljdk-imaging-parallel</t>
   </si>
   <si>
     <t>graaljdk-imaging-single</t>
-  </si>
-  <si>
-    <t>graaljdk-plain</t>
   </si>
   <si>
     <t>openjdk-imaging-parallel</t>
@@ -58,16 +49,10 @@
     <t>openjdk-openimaj</t>
   </si>
   <si>
-    <t>openjdk-plain</t>
-  </si>
-  <si>
     <t>zulu-imaging-parallel</t>
   </si>
   <si>
     <t>zulu-imaging-single</t>
-  </si>
-  <si>
-    <t>zulu-plain</t>
   </si>
   <si>
     <t>python-pure-simple</t>
@@ -101,6 +86,21 @@
   </si>
   <si>
     <t>python-with-opencv</t>
+  </si>
+  <si>
+    <t>adopt-pure</t>
+  </si>
+  <si>
+    <t>amazoncorretto-pure</t>
+  </si>
+  <si>
+    <t>graaljdk-pure</t>
+  </si>
+  <si>
+    <t>openjdk-pure</t>
+  </si>
+  <si>
+    <t>zulu-pure</t>
   </si>
 </sst>
 </file>
@@ -422,9 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -465,79 +463,79 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AA1" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">

</xml_diff>